<commit_message>
page 1 error fix
</commit_message>
<xml_diff>
--- a/inputs/transactions_all/transactions.xlsx
+++ b/inputs/transactions_all/transactions.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q9"/>
+  <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -872,10 +872,8 @@
       <c r="Q8" t="inlineStr"/>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>2021-12-18 10:55:00</t>
-        </is>
+      <c r="A9" s="2" t="n">
+        <v>44548.45486111111</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -922,6 +920,155 @@
       <c r="P9" t="inlineStr"/>
       <c r="Q9" t="inlineStr"/>
     </row>
+    <row r="10">
+      <c r="A10" s="2" t="n">
+        <v>44548.4875</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" t="n">
+        <v>169.93</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="n">
+        <v>169.93</v>
+      </c>
+      <c r="H10" t="n">
+        <v>-169.93</v>
+      </c>
+      <c r="I10" t="n">
+        <v>2</v>
+      </c>
+      <c r="J10" t="n">
+        <v>3</v>
+      </c>
+      <c r="K10" t="n">
+        <v>-680.4399999999998</v>
+      </c>
+      <c r="L10" t="n">
+        <v>-510.5099999999998</v>
+      </c>
+      <c r="M10" t="n">
+        <v>-170.1699999999999</v>
+      </c>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
+      <c r="P10" t="inlineStr"/>
+      <c r="Q10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="n">
+        <v>44548.5</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>AMZN</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" t="n">
+        <v>3354.21</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>3354.21</v>
+      </c>
+      <c r="H11" t="n">
+        <v>-3354.21</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>1</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" t="n">
+        <v>3354.21</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0</v>
+      </c>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
+      <c r="P11" t="inlineStr"/>
+      <c r="Q11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2021-12-18 12:01:00</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>AMZN</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" t="n">
+        <v>3354.21</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" t="n">
+        <v>3354.21</v>
+      </c>
+      <c r="H12" t="n">
+        <v>-3354.21</v>
+      </c>
+      <c r="I12" t="n">
+        <v>1</v>
+      </c>
+      <c r="J12" t="n">
+        <v>2</v>
+      </c>
+      <c r="K12" t="n">
+        <v>3354.21</v>
+      </c>
+      <c r="L12" t="n">
+        <v>6708.42</v>
+      </c>
+      <c r="M12" t="n">
+        <v>3354.21</v>
+      </c>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
+      <c r="P12" t="inlineStr"/>
+      <c r="Q12" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>